<commit_message>
Updated the notebook for one college
</commit_message>
<xml_diff>
--- a/Output - NEET Opening Closing 2020.xlsx
+++ b/Output - NEET Opening Closing 2020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maverick\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Freelancing\VidyarthiMitra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="29">
   <si>
     <t>SC</t>
   </si>
@@ -85,9 +85,6 @@
     <t>S-AIR</t>
   </si>
   <si>
-    <t xml:space="preserve">Sr Code </t>
-  </si>
-  <si>
     <t>College Name</t>
   </si>
   <si>
@@ -110,6 +107,18 @@
   </si>
   <si>
     <t>01101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code </t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>NRI</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -156,10 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,43 +486,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -519,327 +533,396 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>47384</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>552</v>
       </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>180913</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>404</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>22048</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>595</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>32096</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>577</v>
       </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>12268</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>618</v>
       </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>7007</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>635</v>
       </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>12081</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>619</v>
       </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>13670</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>615</v>
       </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>8971</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>629</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>20470</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>599</v>
       </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
+      <c r="G11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>4111</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>649</v>
       </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
+      <c r="G12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>9448</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>627</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>624419</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>164</v>
       </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>33135</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>575</v>
       </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
+      <c r="G15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>